<commit_message>
add comp info home
</commit_message>
<xml_diff>
--- a/Library/Altium_Lib/Yeni eklenen libraryler.xlsx
+++ b/Library/Altium_Lib/Yeni eklenen libraryler.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\AltiumLibrary\AltiumLibrary\Library\Altium_Lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_HW\Altium Lib\Library\Altium_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A2CE26-C164-48B1-9482-F1779D7EFDD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5544F27A-235C-4F5F-BE95-2D77119EB7D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12240" xr2:uid="{359FDF62-FE91-448D-A3D5-0B506578322F}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{359FDF62-FE91-448D-A3D5-0B506578322F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,22 +466,22 @@
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>